<commit_message>
Run SCD0219 - Admin SLN melakukan Modul Mapping and edit excel
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0219 - Admin SLN melakukan Modul Mapping.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0219 - Admin SLN melakukan Modul Mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71643C8-8994-4E2F-B3E4-B1FC98CDCCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AE014C-4EA8-4FF2-8FF5-D7DF1C51898D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0219" sheetId="2" r:id="rId1"/>
@@ -166,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -179,19 +179,28 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -587,39 +596,40 @@
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="11">
         <v>52326</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="11" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="9"/>
+      <c r="Q2" s="13"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -631,8 +641,8 @@
       <c r="C3" s="4"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="7"/>
       <c r="I3" s="3"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="2"/>
@@ -643,8 +653,8 @@
       <c r="C4" s="4"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="7"/>
       <c r="I4" s="3"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="3"/>
@@ -656,8 +666,8 @@
       <c r="C5" s="4"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="5"/>
@@ -665,8 +675,8 @@
       <c r="C6" s="4"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>